<commit_message>
Update dashboard UI: remove borders, fix header backgrounds, improve styling
</commit_message>
<xml_diff>
--- a/frontend/fifty.xlsx
+++ b/frontend/fifty.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Go Live</t>
+          <t>Not Started</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>In Progress</t>
+          <t>Go Live</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>go_live</t>
+          <t>Go Live</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>not_started</t>
+          <t>Go Live</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>not_started</t>
+          <t>Go Live</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>not_started</t>
+          <t>Go Live</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>not_started</t>
+          <t>Go Live</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>go_live</t>
+          <t>not_started</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>go_live</t>
+          <t>not_started</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>go_live</t>
+          <t>not_started</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>go_live</t>
+          <t>not_started</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>go_live</t>
+          <t>not_started</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>go_live</t>
+          <t>not_started</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>go_live</t>
+          <t>not_started</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>not_started</t>
+          <t>Go Live</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>go_live</t>
+          <t>not_started</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>in_progress</t>
+          <t>not_started</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>go_live</t>
+          <t>not_started</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>go_live</t>
+          <t>not_started</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>in_progress</t>
+          <t>not_started</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>In Progress</t>
+          <t>not_started</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>go_live</t>
+          <t>not_started</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Make Unavailable MFI list fully database-driven, add real-time status sync, add MFIStatusHistory model, and update all relevant components.
</commit_message>
<xml_diff>
--- a/frontend/fifty.xlsx
+++ b/frontend/fifty.xlsx
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Go Live</t>
+          <t>Not Started</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Go Live</t>
+          <t>Not Started</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Go Live</t>
+          <t>Not Started</t>
         </is>
       </c>
     </row>

</xml_diff>